<commit_message>
time sheet and attendance updated
</commit_message>
<xml_diff>
--- a/Admin/Gaby/spring/TimeSheet_Week3.xlsx
+++ b/Admin/Gaby/spring/TimeSheet_Week3.xlsx
@@ -364,10 +364,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -613,11 +613,15 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="10"/>
+      <c r="G14" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="I14" s="12" t="n">
         <f aca="false">SUM(B14:H14)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J14" s="8"/>
     </row>
@@ -647,15 +651,15 @@
       </c>
       <c r="G15" s="12" t="n">
         <f aca="false">SUM(G6:G14)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="12" t="n">
         <f aca="false">SUM(H6:H14)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="12" t="n">
         <f aca="false">SUM(I6:I14)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>